<commit_message>
implement the test cases
</commit_message>
<xml_diff>
--- a/src/test/TestCases.xlsx
+++ b/src/test/TestCases.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">A and B are the same File located in different directories.</t>
+  </si>
   <si>
     <t xml:space="preserve">Case #</t>
   </si>
@@ -148,16 +151,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,215 +292,233 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="7.44"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" s="2" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="B10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="B11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="B14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="B15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="B16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" s="5" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="B17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" s="6" customFormat="true" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>5</v>
+      <c r="B18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>